<commit_message>
Oh man, just like so much.
</commit_message>
<xml_diff>
--- a/data/hillsborough_district/personnel_reports_oof/Hillsborough Schools - Personnel Reports OOF.xlsx
+++ b/data/hillsborough_district/personnel_reports_oof/Hillsborough Schools - Personnel Reports OOF.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihodgson/Documents/GitHub/hillsborough_grades/data/hillsborough_district/personnel_reports_oof/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B41EDBAE-CA9C-604A-9767-BBA210223F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF3E0EE-CC9B-314A-8D93-BF47D2C3737D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="500" windowWidth="16800" windowHeight="20500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schools" sheetId="3" r:id="rId1"/>
     <sheet name="Hillsborough Schools - Personne" sheetId="1" r:id="rId2"/>
     <sheet name="Helper" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Schools!$A$1:$B$238</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8289" uniqueCount="2966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8329" uniqueCount="2968">
   <si>
     <t>File Name</t>
   </si>
@@ -8938,12 +8939,18 @@
   </si>
   <si>
     <t>Note: This table lists distinct employee ID / site pairs. We don't want to count a teacher twice if they are OOF at the same school.</t>
+  </si>
+  <si>
+    <t>D/F total</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -9495,9 +9502,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9535,7 +9542,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9641,7 +9648,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9783,18 +9790,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C238"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9802,7 +9809,7 @@
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -9812,8 +9819,14 @@
       <c r="C1" s="3" t="s">
         <v>2964</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>2966</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>886</v>
       </c>
@@ -9824,8 +9837,16 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f>SUMIFS(B:B, C:C, 1)</f>
+        <v>211</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B:B)</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1224</v>
       </c>
@@ -9833,8 +9854,12 @@
         <f>COUNTIF(Helper!B:B, A3)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f>E2/F2</f>
+        <v>0.2060546875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1344</v>
       </c>
@@ -9842,8 +9867,11 @@
         <f>COUNTIF(Helper!B:B, A4)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -9851,8 +9879,12 @@
         <f>COUNTIF(Helper!B:B, A5)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f>F3/F4</f>
+        <v>1.9439121462264151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2055</v>
       </c>
@@ -9861,7 +9893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -9870,7 +9902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>687</v>
       </c>
@@ -9879,7 +9911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>458</v>
       </c>
@@ -9888,7 +9920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -9897,7 +9929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>411</v>
       </c>
@@ -9906,7 +9938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>489</v>
       </c>
@@ -9915,7 +9947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -9924,7 +9956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>866</v>
       </c>
@@ -9933,7 +9965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2096</v>
       </c>
@@ -9942,7 +9974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1006</v>
       </c>
@@ -12043,17 +12075,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1170"/>
   <sheetViews>
-    <sheetView topLeftCell="A1128" workbookViewId="0">
-      <selection activeCell="A1171" sqref="A1171"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42482,23 +42514,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1170"/>
+  <autoFilter ref="A1:H1170" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <hyperlinks>
-    <hyperlink ref="H749" r:id="rId1"/>
-    <hyperlink ref="H204" r:id="rId2"/>
-    <hyperlink ref="H1169" r:id="rId3"/>
-    <hyperlink ref="H801" r:id="rId4"/>
-    <hyperlink ref="H1170" r:id="rId5"/>
+    <hyperlink ref="H749" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H204" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H1169" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="H801" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="H1170" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1025"/>
   <sheetViews>
-    <sheetView topLeftCell="A977" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1025" sqref="B1025"/>
     </sheetView>
   </sheetViews>
@@ -50713,4 +50745,357 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA025E0F-ADA8-A247-A3F4-56ED8A71121A}">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A2)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A3)</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A4)</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A5)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A6)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A7)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A8)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A9)</f>
+        <v>607</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A10)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A11)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A12)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A13)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A14)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A16)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A17)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A18)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>448</v>
+      </c>
+      <c r="B19">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A19)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B20">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A20)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B21">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A21)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B22">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A22)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B23">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B24">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A24)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B25">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A25)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B26">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A26)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B27">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A27)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B28">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B29">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>2957</v>
+      </c>
+      <c r="B30">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B31">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A31)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>2561</v>
+      </c>
+      <c r="B32">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>2595</v>
+      </c>
+      <c r="B33">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>2606</v>
+      </c>
+      <c r="B34">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A34)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B35">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>2699</v>
+      </c>
+      <c r="B36">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A36)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>2708</v>
+      </c>
+      <c r="B37">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A37)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>2766</v>
+      </c>
+      <c r="B38">
+        <f>COUNTIF('Hillsborough Schools - Personne'!F:F, Sheet1!A38)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>